<commit_message>
Added Header tab to the RestShell Worksheet. Still cleaning up the JSON formatting, but references to cells seem to be working now.
</commit_message>
<xml_diff>
--- a/Restshell_Worksheet.xlsx
+++ b/Restshell_Worksheet.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SunReyEagle\Projects\RestShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B40D1F-E15F-404A-9E04-8E8939CBA706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FC8322-2B36-4B70-8E27-EA7C9C28F932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82BAB86A-2659-457E-AB24-15E7C625509F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{82BAB86A-2659-457E-AB24-15E7C625509F}"/>
   </bookViews>
   <sheets>
     <sheet name="Requests" sheetId="1" r:id="rId1"/>
-    <sheet name="Export" sheetId="2" r:id="rId2"/>
+    <sheet name="Headers" sheetId="3" r:id="rId2"/>
+    <sheet name="Export" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,8 +37,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Title</t>
   </si>
@@ -76,9 +99,6 @@
   </si>
   <si>
     <t>Example_file.json</t>
-  </si>
-  <si>
-    <t>{ "im a" : "JSON" }</t>
   </si>
   <si>
     <t>File_data_to_send.txt</t>
@@ -114,6 +134,69 @@
   </si>
   <si>
     <t>Export as Series Functions</t>
+  </si>
+  <si>
+    <t>{ "JSON" : "Bourne" }</t>
+  </si>
+  <si>
+    <t>Header Names</t>
+  </si>
+  <si>
+    <t>Header Values</t>
+  </si>
+  <si>
+    <t>Content-Type</t>
+  </si>
+  <si>
+    <t>Accept</t>
+  </si>
+  <si>
+    <t>application/html</t>
+  </si>
+  <si>
+    <t>*/*</t>
+  </si>
+  <si>
+    <t>application/json</t>
+  </si>
+  <si>
+    <t>application/pdf</t>
+  </si>
+  <si>
+    <t>application/x-www-form-urlencoded</t>
+  </si>
+  <si>
+    <t>text/xml</t>
+  </si>
+  <si>
+    <t>text/html</t>
+  </si>
+  <si>
+    <t>audio/mpeg</t>
+  </si>
+  <si>
+    <t>video/mp4</t>
+  </si>
+  <si>
+    <t>image/jpeg</t>
+  </si>
+  <si>
+    <t>Common Content Type/Accept Options</t>
+  </si>
+  <si>
+    <t>text/json</t>
+  </si>
+  <si>
+    <t>Header Code</t>
+  </si>
+  <si>
+    <t>Header Group</t>
+  </si>
+  <si>
+    <t>debug</t>
+  </si>
+  <si>
+    <t>debug index</t>
   </si>
 </sst>
 </file>
@@ -176,7 +259,22 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -200,30 +298,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AEDFD834-3442-4AE8-B443-1327BCC55E80}" name="Table1" displayName="Table1" ref="A1:G5" totalsRowShown="0">
-  <autoFilter ref="A1:G5" xr:uid="{AEDFD834-3442-4AE8-B443-1327BCC55E80}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AEDFD834-3442-4AE8-B443-1327BCC55E80}" name="Table1" displayName="Table1" ref="A1:I5" totalsRowShown="0">
+  <autoFilter ref="A1:I5" xr:uid="{AEDFD834-3442-4AE8-B443-1327BCC55E80}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D07728D8-7F6A-4B3F-85E6-43CA92E421B1}" name="Request Title"/>
     <tableColumn id="2" xr3:uid="{B7B35981-BE54-48F6-8A69-727F781A7ACA}" name="TargetURL" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{CCD51A27-A85D-4724-B491-87B55D02531E}" name="HTTP_Method"/>
-    <tableColumn id="4" xr3:uid="{9F53C059-1728-4CEB-BB68-21EC76B024AD}" name="Headers"/>
+    <tableColumn id="4" xr3:uid="{9F53C059-1728-4CEB-BB68-21EC76B024AD}" name="Headers" dataDxfId="3">
+      <calculatedColumnFormula>INDEX(Table3[[#This Row],[Header Code]], MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0))</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="5" xr3:uid="{ED78A8B1-A11F-4A18-9D32-E15C61CBEA2E}" name="Request_Body"/>
     <tableColumn id="6" xr3:uid="{67C8EE67-DBF3-48F5-B942-78F24D3600D1}" name="Request_Body_FileName"/>
     <tableColumn id="7" xr3:uid="{744E10C1-2A32-4E95-9F36-53926701240E}" name="Output_Filename"/>
+    <tableColumn id="10" xr3:uid="{C99C617F-0505-49E3-BF02-C95CD0F5B4A8}" name="debug" dataDxfId="1">
+      <calculatedColumnFormula>MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{FB4D6269-A10D-4421-8A2A-CDC4555E8C55}" name="debug index" dataDxfId="0">
+      <calculatedColumnFormula array="1">INDEX(Headers!$A$2:$E$6, Table1[[#This Row],[debug]],5)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1F0A502C-D2A6-4C34-921E-AEB6142FDE67}" name="Table3" displayName="Table3" ref="A1:E5" totalsRowShown="0">
+  <autoFilter ref="A1:E5" xr:uid="{1F0A502C-D2A6-4C34-921E-AEB6142FDE67}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2933AE7E-E153-4D8E-BA6E-A838EA227F8D}" name="Request Title"/>
+    <tableColumn id="2" xr3:uid="{EAC99EB9-981E-45D6-B455-9859A4E22321}" name="Header Names"/>
+    <tableColumn id="3" xr3:uid="{4B700452-AF33-4C78-883D-994C3A548C25}" name="Header Values"/>
+    <tableColumn id="4" xr3:uid="{4E0443DB-C9C1-47C1-95E7-349C72F7A35D}" name="Header Code" dataDxfId="4">
+      <calculatedColumnFormula>_xlfn.CONCAT("""", Table3[[#This Row],[Header Names]], ","": """, Table3[[#This Row],[Header Values]], """")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{3BA627B5-F18B-4181-BDF7-38B65F035A59}" name="Header Group" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.TEXTJOIN(",", TRUE,D2:D3)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E19BDE79-9B40-4DEC-9B23-FF5403DA25E3}" name="Table4" displayName="Table4" ref="H1:H11" totalsRowShown="0">
+  <autoFilter ref="H1:H11" xr:uid="{E19BDE79-9B40-4DEC-9B23-FF5403DA25E3}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{5EC9F642-77AB-48DC-9D28-10A9FDDFEADC}" name="Common Content Type/Accept Options"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B44E67D8-9075-4173-8BEA-34772107489A}" name="Table2" displayName="Table2" ref="A1:L6" totalsRowShown="0">
   <autoFilter ref="A1:L6" xr:uid="{B44E67D8-9075-4173-8BEA-34772107489A}"/>
   <tableColumns count="12">
-    <tableColumn id="12" xr3:uid="{E6FAA3AB-63E2-4FDF-BC8F-E5AA90AFEA27}" name="Export as Series" dataDxfId="2">
+    <tableColumn id="12" xr3:uid="{E6FAA3AB-63E2-4FDF-BC8F-E5AA90AFEA27}" name="Export as Series" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.CONCAT(Table2[Export as Series Functions])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{F92B5F86-D79A-4034-A273-A5310A368DA6}" name="Export as Series Functions" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{024017C8-B9FE-4068-A08A-BF156772955D}" name="Export as RestShell JSON" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F92B5F86-D79A-4034-A273-A5310A368DA6}" name="Export as Series Functions" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{024017C8-B9FE-4068-A08A-BF156772955D}" name="Export as RestShell JSON" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{CF17ED99-C650-4A8A-9877-FBA68EC96552}" name="Title"/>
     <tableColumn id="4" xr3:uid="{119E6705-9EA8-4E35-B49B-F34D5DAA1045}" name="TargetURL"/>
     <tableColumn id="5" xr3:uid="{D5A155B7-7C2C-4622-AAE4-40EC04918CA7}" name="HTTP_Method"/>
@@ -555,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F37D43-4435-4ACF-9D1B-346079C72D6A}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,13 +700,15 @@
     <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -594,8 +730,14 @@
       <c r="G1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -605,16 +747,28 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
+      <c r="D2" t="str">
+        <f>INDEX(Headers!$A$2:$E$6, MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0),5)</f>
+        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
+      </c>
       <c r="F2" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" t="str" cm="1">
+        <f t="array" ref="I2">INDEX(Headers!$A$2:$E$6, Table1[[#This Row],[debug]],5)</f>
+        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -622,21 +776,49 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
+      <c r="D3" t="str">
+        <f>INDEX(Headers!$A$2:$E$6, MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0),5)</f>
+        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
+      </c>
       <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0)</f>
+        <v>3</v>
+      </c>
+      <c r="I3" t="str" cm="1">
+        <f t="array" ref="I3">INDEX(Headers!$A$2:$E$6, Table1[[#This Row],[debug]],5)</f>
+        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="e">
+        <f>MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I4" t="e" cm="1">
+        <f t="array" ref="I4">INDEX(Headers!$A$2:$E$6, Table1[[#This Row],[debug]],5)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
+      <c r="H5" t="e">
+        <f>MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I5" t="e" cm="1">
+        <f t="array" ref="I5">INDEX(Headers!$A$2:$E$6, Table1[[#This Row],[debug]],5)</f>
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -652,17 +834,183 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A157AD85-9A01-4FAB-8DC7-CE68C94B7E52}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="str">
+        <f>_xlfn.CONCAT("""", Table3[[#This Row],[Header Names]], ","": """, Table3[[#This Row],[Header Values]], """")</f>
+        <v>"Content-Type,": "application/html"</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E5" si="0">_xlfn.TEXTJOIN(",", TRUE,D2:D3)</f>
+        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xlfn.CONCAT("""", Table3[[#This Row],[Header Names]], ","": """, Table3[[#This Row],[Header Values]], """")</f>
+        <v>"Accept,": "*/*"</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>"Accept,": "*/*","Content-Type,": "application/html"</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="str">
+        <f>_xlfn.CONCAT("""", Table3[[#This Row],[Header Names]], ","": """, Table3[[#This Row],[Header Values]], """")</f>
+        <v>"Content-Type,": "application/html"</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="str">
+        <f>_xlfn.CONCAT("""", Table3[[#This Row],[Header Names]], ","": """, Table3[[#This Row],[Header Values]], """")</f>
+        <v>"Accept,": "*/*"</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>"Accept,": "*/*"</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F5048BA-D6CF-4DE3-AC00-1A9A01F57E38}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.7109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="66.7109375" customWidth="1"/>
     <col min="3" max="3" width="70.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="62.5703125" customWidth="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
@@ -677,13 +1025,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -707,20 +1055,47 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="330" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f>_xlfn.CONCAT(Table2[Export as Series Functions])</f>
         <v>{     "Requests": [{
 "Title": "Simple Worksheet Example Request", 
 "TargetURL": "www.google.com", 
 "HTTP_Method": "GET", 
-"Headers": "", 
+"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
+"Request_Body": "", 
+"Request_Body_FileName": "Example_file.json", 
+"Output_Filename": "response.txt", 
+"EndNote": "--------------------------------------------"
+}{
+"Title": "Another Example", 
+"TargetURL": "www.google.com", 
+"HTTP_Method": "GET", 
+"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
+"Request_Body": "{ "JSON" : "Bourne" }", 
+"Request_Body_FileName": "File_data_to_send.txt", 
+"Output_Filename": "response.txt", 
+"EndNote": "--------------------------------------------"
+}]}</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="str">
+        <f>_xlfn.TEXTJOIN( ",",TRUE,Table2[Export as Series Functions])</f>
+        <v>{     "Requests": [,{
+"Title": "Simple Worksheet Example Request", 
+"TargetURL": "www.google.com", 
+"HTTP_Method": "GET", 
+"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
 "Request_Body": "", 
 "Request_Body_FileName": "Example_file.json", 
 "Output_Filename": "response.txt", 
@@ -729,39 +1104,12 @@
 "Title": "Another Example", 
 "TargetURL": "www.google.com", 
 "HTTP_Method": "GET", 
-"Headers": "", 
-"Request_Body": "{ "im a" : "JSON" }", 
+"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
+"Request_Body": "{ "JSON" : "Bourne" }", 
 "Request_Body_FileName": "File_data_to_send.txt", 
 "Output_Filename": "response.txt", 
 "EndNote": "--------------------------------------------"
-}]}</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="str">
-        <f>_xlfn.CONCAT(Table2[Export as Series Functions])</f>
-        <v>{     "Requests": [{
-"Title": "Simple Worksheet Example Request", 
-"TargetURL": "www.google.com", 
-"HTTP_Method": "GET", 
-"Headers": "", 
-"Request_Body": "", 
-"Request_Body_FileName": "Example_file.json", 
-"Output_Filename": "response.txt", 
-"EndNote": "--------------------------------------------"
-},{
-"Title": "Another Example", 
-"TargetURL": "www.google.com", 
-"HTTP_Method": "GET", 
-"Headers": "", 
-"Request_Body": "{ "im a" : "JSON" }", 
-"Request_Body_FileName": "File_data_to_send.txt", 
-"Output_Filename": "response.txt", 
-"EndNote": "--------------------------------------------"
-}]}</v>
+},]}</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>_xlfn.CONCAT("{", $K$3, D3, E3, F3, G3, H3, I3, J3, L3)</f>
@@ -769,7 +1117,7 @@
 "Title": "Simple Worksheet Example Request", 
 "TargetURL": "www.google.com", 
 "HTTP_Method": "GET", 
-"Headers": "", 
+"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
 "Request_Body": "", 
 "Request_Body_FileName": "Example_file.json", 
 "Output_Filename": "response.txt", 
@@ -782,7 +1130,7 @@
 "Title": "Simple Worksheet Example Request", 
 "TargetURL": "www.google.com", 
 "HTTP_Method": "GET", 
-"Headers": "", 
+"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
 "Request_Body": "", 
 "Request_Body_FileName": "Example_file.json", 
 "Output_Filename": "response.txt", 
@@ -806,7 +1154,7 @@
       </c>
       <c r="G3" s="3" t="str">
         <f>_xlfn.CONCAT( """",$G$1,""": """, Requests!D2, """, ", $K$3)</f>
-        <v xml:space="preserve">"Headers": "", 
+        <v xml:space="preserve">"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
 </v>
       </c>
       <c r="H3" s="3" t="str">
@@ -825,21 +1173,21 @@
 </v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="str">
-        <f>_xlfn.CONCAT(",{", $K$3, D4, E4, F4, G4, H4, I4, J4, L4)</f>
-        <v>,{
+        <f>_xlfn.CONCAT("{", $K$3, D4, E4, F4, G4, H4, I4, J4, L4)</f>
+        <v>{
 "Title": "Another Example", 
 "TargetURL": "www.google.com", 
 "HTTP_Method": "GET", 
-"Headers": "", 
-"Request_Body": "{ "im a" : "JSON" }", 
+"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
+"Request_Body": "{ "JSON" : "Bourne" }", 
 "Request_Body_FileName": "File_data_to_send.txt", 
 "Output_Filename": "response.txt", 
 "EndNote": "--------------------------------------------"
@@ -851,8 +1199,8 @@
 "Title": "Another Example", 
 "TargetURL": "www.google.com", 
 "HTTP_Method": "GET", 
-"Headers": "", 
-"Request_Body": "{ "im a" : "JSON" }", 
+"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
+"Request_Body": "{ "JSON" : "Bourne" }", 
 "Request_Body_FileName": "File_data_to_send.txt", 
 "Output_Filename": "response.txt", 
 "EndNote": "--------------------------------------------"
@@ -875,12 +1223,12 @@
       </c>
       <c r="G4" s="3" t="str">
         <f>_xlfn.CONCAT( """",$G$1,""": """, Requests!D3, """, ", $K$3)</f>
-        <v xml:space="preserve">"Headers": "", 
+        <v xml:space="preserve">"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
 </v>
       </c>
       <c r="H4" s="3" t="str">
         <f>_xlfn.CONCAT( """",$H$1,""": """, Requests!E3, """, ", $K$3)</f>
-        <v xml:space="preserve">"Request_Body": "{ "im a" : "JSON" }", 
+        <v xml:space="preserve">"Request_Body": "{ "JSON" : "Bourne" }", 
 </v>
       </c>
       <c r="I4" s="3" t="str">
@@ -894,15 +1242,15 @@
 </v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated the RestShell worksheet to handle the Headers. Headers format looks good, still need to find a clean way to export it without CSV escape quotes.
</commit_message>
<xml_diff>
--- a/Restshell_Worksheet.xlsx
+++ b/Restshell_Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SunReyEagle\Projects\RestShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FC8322-2B36-4B70-8E27-EA7C9C28F932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF071576-B473-4AAB-A5BC-D91263764513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{82BAB86A-2659-457E-AB24-15E7C625509F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{82BAB86A-2659-457E-AB24-15E7C625509F}"/>
   </bookViews>
   <sheets>
     <sheet name="Requests" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>Title</t>
   </si>
@@ -123,22 +123,13 @@
     <t>EndNote</t>
   </si>
   <si>
-    <t>{     "Requests": [</t>
-  </si>
-  <si>
     <t>"EndNote": "--------------------------------------------"
 }</t>
   </si>
   <si>
-    <t>]}</t>
-  </si>
-  <si>
     <t>Export as Series Functions</t>
   </si>
   <si>
-    <t>{ "JSON" : "Bourne" }</t>
-  </si>
-  <si>
     <t>Header Names</t>
   </si>
   <si>
@@ -197,6 +188,9 @@
   </si>
   <si>
     <t>debug index</t>
+  </si>
+  <si>
+    <t>{\"JSON\" : \"Bourne\" }</t>
   </si>
 </sst>
 </file>
@@ -267,7 +261,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -276,10 +273,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -304,16 +298,16 @@
     <tableColumn id="1" xr3:uid="{D07728D8-7F6A-4B3F-85E6-43CA92E421B1}" name="Request Title"/>
     <tableColumn id="2" xr3:uid="{B7B35981-BE54-48F6-8A69-727F781A7ACA}" name="TargetURL" dataCellStyle="Hyperlink"/>
     <tableColumn id="3" xr3:uid="{CCD51A27-A85D-4724-B491-87B55D02531E}" name="HTTP_Method"/>
-    <tableColumn id="4" xr3:uid="{9F53C059-1728-4CEB-BB68-21EC76B024AD}" name="Headers" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{9F53C059-1728-4CEB-BB68-21EC76B024AD}" name="Headers" dataDxfId="7">
       <calculatedColumnFormula>INDEX(Table3[[#This Row],[Header Code]], MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{ED78A8B1-A11F-4A18-9D32-E15C61CBEA2E}" name="Request_Body"/>
     <tableColumn id="6" xr3:uid="{67C8EE67-DBF3-48F5-B942-78F24D3600D1}" name="Request_Body_FileName"/>
     <tableColumn id="7" xr3:uid="{744E10C1-2A32-4E95-9F36-53926701240E}" name="Output_Filename"/>
-    <tableColumn id="10" xr3:uid="{C99C617F-0505-49E3-BF02-C95CD0F5B4A8}" name="debug" dataDxfId="1">
+    <tableColumn id="10" xr3:uid="{C99C617F-0505-49E3-BF02-C95CD0F5B4A8}" name="debug" dataDxfId="6">
       <calculatedColumnFormula>MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{FB4D6269-A10D-4421-8A2A-CDC4555E8C55}" name="debug index" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{FB4D6269-A10D-4421-8A2A-CDC4555E8C55}" name="debug index" dataDxfId="5">
       <calculatedColumnFormula array="1">INDEX(Headers!$A$2:$E$6, Table1[[#This Row],[debug]],5)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -328,11 +322,11 @@
     <tableColumn id="1" xr3:uid="{2933AE7E-E153-4D8E-BA6E-A838EA227F8D}" name="Request Title"/>
     <tableColumn id="2" xr3:uid="{EAC99EB9-981E-45D6-B455-9859A4E22321}" name="Header Names"/>
     <tableColumn id="3" xr3:uid="{4B700452-AF33-4C78-883D-994C3A548C25}" name="Header Values"/>
-    <tableColumn id="4" xr3:uid="{4E0443DB-C9C1-47C1-95E7-349C72F7A35D}" name="Header Code" dataDxfId="4">
-      <calculatedColumnFormula>_xlfn.CONCAT("""", Table3[[#This Row],[Header Names]], ","": """, Table3[[#This Row],[Header Values]], """")</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{4E0443DB-C9C1-47C1-95E7-349C72F7A35D}" name="Header Code" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.CONCAT("{", CHAR(34), "Name", CHAR(34), ":", CHAR(34), Table3[[#This Row],[Header Names]], CHAR(34), ",", CHAR(34), "Value", CHAR(34), ":", CHAR(34), Table3[[#This Row],[Header Values]], CHAR(34), "}")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3BA627B5-F18B-4181-BDF7-38B65F035A59}" name="Header Group" dataDxfId="2">
-      <calculatedColumnFormula>_xlfn.TEXTJOIN(",", TRUE,D2:D3)</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{3BA627B5-F18B-4181-BDF7-38B65F035A59}" name="Header Group" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("[", _xlfn.TEXTJOIN(",", TRUE,D2:D3), "]")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -350,14 +344,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B44E67D8-9075-4173-8BEA-34772107489A}" name="Table2" displayName="Table2" ref="A1:L6" totalsRowShown="0">
-  <autoFilter ref="A1:L6" xr:uid="{B44E67D8-9075-4173-8BEA-34772107489A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B44E67D8-9075-4173-8BEA-34772107489A}" name="Table2" displayName="Table2" ref="A1:L5" totalsRowShown="0">
+  <autoFilter ref="A1:L5" xr:uid="{B44E67D8-9075-4173-8BEA-34772107489A}"/>
   <tableColumns count="12">
-    <tableColumn id="12" xr3:uid="{E6FAA3AB-63E2-4FDF-BC8F-E5AA90AFEA27}" name="Export as Series" dataDxfId="7">
+    <tableColumn id="12" xr3:uid="{E6FAA3AB-63E2-4FDF-BC8F-E5AA90AFEA27}" name="Export as Series" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.CONCAT(Table2[Export as Series Functions])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{F92B5F86-D79A-4034-A273-A5310A368DA6}" name="Export as Series Functions" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{024017C8-B9FE-4068-A08A-BF156772955D}" name="Export as RestShell JSON" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{F92B5F86-D79A-4034-A273-A5310A368DA6}" name="Export as Series Functions" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{024017C8-B9FE-4068-A08A-BF156772955D}" name="Export as RestShell JSON" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{CF17ED99-C650-4A8A-9877-FBA68EC96552}" name="Title"/>
     <tableColumn id="4" xr3:uid="{119E6705-9EA8-4E35-B49B-F34D5DAA1045}" name="TargetURL"/>
     <tableColumn id="5" xr3:uid="{D5A155B7-7C2C-4622-AAE4-40EC04918CA7}" name="HTTP_Method"/>
@@ -692,23 +686,23 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -731,13 +725,13 @@
         <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -749,7 +743,7 @@
       </c>
       <c r="D2" t="str">
         <f>INDEX(Headers!$A$2:$E$6, MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0),5)</f>
-        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
+        <v>[{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}]</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -763,10 +757,10 @@
       </c>
       <c r="I2" t="str" cm="1">
         <f t="array" ref="I2">INDEX(Headers!$A$2:$E$6, Table1[[#This Row],[debug]],5)</f>
-        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>[{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}]</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -778,10 +772,10 @@
       </c>
       <c r="D3" t="str">
         <f>INDEX(Headers!$A$2:$E$6, MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0),5)</f>
-        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
+        <v>[{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}]</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -795,10 +789,10 @@
       </c>
       <c r="I3" t="str" cm="1">
         <f t="array" ref="I3">INDEX(Headers!$A$2:$E$6, Table1[[#This Row],[debug]],5)</f>
-        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>[{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}]</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="H4" t="e">
         <f>MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0)</f>
@@ -809,7 +803,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="H5" t="e">
         <f>MATCH(Table1[[#This Row],[Request Title]],Table3[Request Title],0)</f>
@@ -835,158 +829,164 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A157AD85-9A01-4FAB-8DC7-CE68C94B7E52}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="str">
+        <f>_xlfn.CONCAT("{", CHAR(34), "Name", CHAR(34), ":", CHAR(34), Table3[[#This Row],[Header Names]], CHAR(34), ",", CHAR(34), "Value", CHAR(34), ":", CHAR(34), Table3[[#This Row],[Header Values]], CHAR(34), "}")</f>
+        <v>{"Name":"Content-Type","Value":"application/html"}</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E5" si="0">_xlfn.CONCAT("[", _xlfn.TEXTJOIN(",", TRUE,D2:D3), "]")</f>
+        <v>[{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}]</v>
+      </c>
+      <c r="H2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="str">
-        <f>_xlfn.CONCAT("""", Table3[[#This Row],[Header Names]], ","": """, Table3[[#This Row],[Header Values]], """")</f>
-        <v>"Content-Type,": "application/html"</v>
-      </c>
-      <c r="E2" t="str">
-        <f t="shared" ref="E2:E5" si="0">_xlfn.TEXTJOIN(",", TRUE,D2:D3)</f>
-        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3" t="str">
-        <f>_xlfn.CONCAT("""", Table3[[#This Row],[Header Names]], ","": """, Table3[[#This Row],[Header Values]], """")</f>
-        <v>"Accept,": "*/*"</v>
+        <f>_xlfn.CONCAT("{", CHAR(34), "Name", CHAR(34), ":", CHAR(34), Table3[[#This Row],[Header Names]], CHAR(34), ",", CHAR(34), "Value", CHAR(34), ":", CHAR(34), Table3[[#This Row],[Header Values]], CHAR(34), "}")</f>
+        <v>{"Name":"Accept","Value":"*/*"}</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" si="0"/>
-        <v>"Accept,": "*/*","Content-Type,": "application/html"</v>
+        <v>[{"Name":"Accept","Value":"*/*"},{"Name":"Content-Type","Value":"application/html"}]</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D4" t="str">
-        <f>_xlfn.CONCAT("""", Table3[[#This Row],[Header Names]], ","": """, Table3[[#This Row],[Header Values]], """")</f>
-        <v>"Content-Type,": "application/html"</v>
+        <f>_xlfn.CONCAT("{", CHAR(34), "Name", CHAR(34), ":", CHAR(34), Table3[[#This Row],[Header Names]], CHAR(34), ",", CHAR(34), "Value", CHAR(34), ":", CHAR(34), Table3[[#This Row],[Header Values]], CHAR(34), "}")</f>
+        <v>{"Name":"Content-Type","Value":"application/html"}</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>"Content-Type,": "application/html","Accept,": "*/*"</v>
+        <v>[{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}]</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D5" t="str">
-        <f>_xlfn.CONCAT("""", Table3[[#This Row],[Header Names]], ","": """, Table3[[#This Row],[Header Values]], """")</f>
-        <v>"Accept,": "*/*"</v>
+        <f>_xlfn.CONCAT("{", CHAR(34), "Name", CHAR(34), ":", CHAR(34), Table3[[#This Row],[Header Names]], CHAR(34), ",", CHAR(34), "Value", CHAR(34), ":", CHAR(34), Table3[[#This Row],[Header Values]], CHAR(34), "}")</f>
+        <v>{"Name":"Accept","Value":"*/*"}</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>"Accept,": "*/*"</v>
+        <v>[{"Name":"Accept","Value":"*/*"}]</v>
       </c>
       <c r="H5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H6" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H7" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H8" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H11" t="s">
-        <v>38</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D12" t="str">
+        <f>CHAR(34)</f>
+        <v>"</v>
       </c>
     </row>
   </sheetData>
@@ -1001,34 +1001,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F5048BA-D6CF-4DE3-AC00-1A9A01F57E38}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.7109375" customWidth="1"/>
-    <col min="3" max="3" width="70.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="62.5703125" customWidth="1"/>
+    <col min="1" max="1" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" customWidth="1"/>
+    <col min="3" max="3" width="70.88671875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="62.5546875" customWidth="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>16</v>
@@ -1061,41 +1061,96 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="176.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="str">
-        <f>_xlfn.CONCAT(Table2[Export as Series Functions])</f>
+        <f>_xlfn.CONCAT("{     ""Requests"": [", _xlfn.TEXTJOIN( ",",TRUE,$B$2:B2), "] }")</f>
         <v>{     "Requests": [{
 "Title": "Simple Worksheet Example Request", 
 "TargetURL": "www.google.com", 
 "HTTP_Method": "GET", 
-"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
+"Headers": [{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}], 
 "Request_Body": "", 
 "Request_Body_FileName": "Example_file.json", 
 "Output_Filename": "response.txt", 
 "EndNote": "--------------------------------------------"
-}{
-"Title": "Another Example", 
-"TargetURL": "www.google.com", 
-"HTTP_Method": "GET", 
-"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
-"Request_Body": "{ "JSON" : "Bourne" }", 
-"Request_Body_FileName": "File_data_to_send.txt", 
-"Output_Filename": "response.txt", 
-"EndNote": "--------------------------------------------"
-}]}</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="176.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="str">
-        <f>_xlfn.TEXTJOIN( ",",TRUE,Table2[Export as Series Functions])</f>
-        <v>{     "Requests": [,{
+}] }</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>TRIM(_xlfn.CONCAT("{", $K$2, D2, E2, F2, G2, H2, I2, J2, L2))</f>
+        <v>{
 "Title": "Simple Worksheet Example Request", 
 "TargetURL": "www.google.com", 
 "HTTP_Method": "GET", 
-"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
+"Headers": [{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}], 
+"Request_Body": "", 
+"Request_Body_FileName": "Example_file.json", 
+"Output_Filename": "response.txt", 
+"EndNote": "--------------------------------------------"
+}</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>_xlfn.CONCAT("{     ""Requests"": [", "{", $K$2, D2, E2, F2, G2, H2, I2, J2, L2," ] }")</f>
+        <v>{     "Requests": [{
+"Title": "Simple Worksheet Example Request", 
+"TargetURL": "www.google.com", 
+"HTTP_Method": "GET", 
+"Headers": [{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}], 
+"Request_Body": "", 
+"Request_Body_FileName": "Example_file.json", 
+"Output_Filename": "response.txt", 
+"EndNote": "--------------------------------------------"
+} ] }</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$D$1,""": """, Requests!A2, """, ", $K$2)</f>
+        <v xml:space="preserve">"Title": "Simple Worksheet Example Request", 
+</v>
+      </c>
+      <c r="E2" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$E$1,""": """, Requests!B2, """, ", $K$2)</f>
+        <v xml:space="preserve">"TargetURL": "www.google.com", 
+</v>
+      </c>
+      <c r="F2" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$F$1,""": """, Requests!C2, """, ", $K$2)</f>
+        <v xml:space="preserve">"HTTP_Method": "GET", 
+</v>
+      </c>
+      <c r="G2" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$G$1,""": ", Requests!D2, ", ", $K$2)</f>
+        <v xml:space="preserve">"Headers": [{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}], 
+</v>
+      </c>
+      <c r="H2" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$H$1,""": """, Requests!E2, """, ", $K$2)</f>
+        <v xml:space="preserve">"Request_Body": "", 
+</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$I$1,""": """, Requests!F2, """, ", $K$2)</f>
+        <v xml:space="preserve">"Request_Body_FileName": "Example_file.json", 
+</v>
+      </c>
+      <c r="J2" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$J$1,""": """, Requests!G2, """, ", $K$2)</f>
+        <v xml:space="preserve">"Output_Filename": "response.txt", 
+</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="str">
+        <f>_xlfn.CONCAT("{", CHAR(13), "  ", CHAR(34),"Requests", CHAR(34), ": [", _xlfn.TEXTJOIN( ",",TRUE,$B$2:B3), "] }")</f>
+        <v>{_x000D_  "Requests": [{
+"Title": "Simple Worksheet Example Request", 
+"TargetURL": "www.google.com", 
+"HTTP_Method": "GET", 
+"Headers": [{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}], 
 "Request_Body": "", 
 "Request_Body_FileName": "Example_file.json", 
 "Output_Filename": "response.txt", 
@@ -1104,157 +1159,83 @@
 "Title": "Another Example", 
 "TargetURL": "www.google.com", 
 "HTTP_Method": "GET", 
-"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
-"Request_Body": "{ "JSON" : "Bourne" }", 
+"Headers": [{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}], 
+"Request_Body": "{\"JSON\" : \"Bourne\" }", 
 "Request_Body_FileName": "File_data_to_send.txt", 
 "Output_Filename": "response.txt", 
 "EndNote": "--------------------------------------------"
-},]}</v>
+}] }</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f>_xlfn.CONCAT("{", $K$3, D3, E3, F3, G3, H3, I3, J3, L3)</f>
-        <v>{
-"Title": "Simple Worksheet Example Request", 
-"TargetURL": "www.google.com", 
-"HTTP_Method": "GET", 
-"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
-"Request_Body": "", 
-"Request_Body_FileName": "Example_file.json", 
-"Output_Filename": "response.txt", 
-"EndNote": "--------------------------------------------"
-}</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <f>_xlfn.CONCAT("{     ""Requests"": [", "{", $K$3, D3, E3, F3, G3, H3, I3, J3, L3," ] }")</f>
-        <v>{     "Requests": [{
-"Title": "Simple Worksheet Example Request", 
-"TargetURL": "www.google.com", 
-"HTTP_Method": "GET", 
-"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
-"Request_Body": "", 
-"Request_Body_FileName": "Example_file.json", 
-"Output_Filename": "response.txt", 
-"EndNote": "--------------------------------------------"
-} ] }</v>
-      </c>
-      <c r="D3" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$D$1,""": """, Requests!A2, """, ", $K$3)</f>
-        <v xml:space="preserve">"Title": "Simple Worksheet Example Request", 
-</v>
-      </c>
-      <c r="E3" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$E$1,""": """, Requests!B2, """, ", $K$3)</f>
-        <v xml:space="preserve">"TargetURL": "www.google.com", 
-</v>
-      </c>
-      <c r="F3" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$F$1,""": """, Requests!C2, """, ", $K$3)</f>
-        <v xml:space="preserve">"HTTP_Method": "GET", 
-</v>
-      </c>
-      <c r="G3" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$G$1,""": """, Requests!D2, """, ", $K$3)</f>
-        <v xml:space="preserve">"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
-</v>
-      </c>
-      <c r="H3" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$H$1,""": """, Requests!E2, """, ", $K$3)</f>
-        <v xml:space="preserve">"Request_Body": "", 
-</v>
-      </c>
-      <c r="I3" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$I$1,""": """, Requests!F2, """, ", $K$3)</f>
-        <v xml:space="preserve">"Request_Body_FileName": "Example_file.json", 
-</v>
-      </c>
-      <c r="J3" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$J$1,""": """, Requests!G2, """, ", $K$3)</f>
-        <v xml:space="preserve">"Output_Filename": "response.txt", 
-</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="150" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="str">
-        <f>_xlfn.CONCAT("{", $K$3, D4, E4, F4, G4, H4, I4, J4, L4)</f>
+        <f>_xlfn.CONCAT("{", $K$2, D3, E3, F3, G3, H3, I3, J3, L3)</f>
         <v>{
 "Title": "Another Example", 
 "TargetURL": "www.google.com", 
 "HTTP_Method": "GET", 
-"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
-"Request_Body": "{ "JSON" : "Bourne" }", 
+"Headers": [{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}], 
+"Request_Body": "{\"JSON\" : \"Bourne\" }", 
 "Request_Body_FileName": "File_data_to_send.txt", 
 "Output_Filename": "response.txt", 
 "EndNote": "--------------------------------------------"
 }</v>
       </c>
-      <c r="C4" s="5" t="str">
-        <f>_xlfn.CONCAT("{     ""Requests"": [", "{", $K$3, D4, E4, F4, G4, H4, I4, J4, L4, " ] }")</f>
+      <c r="C3" s="5" t="str">
+        <f>_xlfn.CONCAT("{     ""Requests"": [", "{", $K$2, D3, E3, F3, G3, H3, I3, J3, L3, " ] }")</f>
         <v>{     "Requests": [{
 "Title": "Another Example", 
 "TargetURL": "www.google.com", 
 "HTTP_Method": "GET", 
-"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
-"Request_Body": "{ "JSON" : "Bourne" }", 
+"Headers": [{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}], 
+"Request_Body": "{\"JSON\" : \"Bourne\" }", 
 "Request_Body_FileName": "File_data_to_send.txt", 
 "Output_Filename": "response.txt", 
 "EndNote": "--------------------------------------------"
 } ] }</v>
       </c>
-      <c r="D4" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$D$1,""": """, Requests!A3, """, ", $K$3)</f>
+      <c r="D3" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$D$1,""": """, Requests!A3, """, ", $K$2)</f>
         <v xml:space="preserve">"Title": "Another Example", 
 </v>
       </c>
-      <c r="E4" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$E$1,""": """, Requests!B3, """, ", $K$3)</f>
+      <c r="E3" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$E$1,""": """, Requests!B3, """, ", $K$2)</f>
         <v xml:space="preserve">"TargetURL": "www.google.com", 
 </v>
       </c>
-      <c r="F4" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$F$1,""": """, Requests!C3, """, ", $K$3)</f>
+      <c r="F3" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$F$1,""": """, Requests!C3, """, ", $K$2)</f>
         <v xml:space="preserve">"HTTP_Method": "GET", 
 </v>
       </c>
-      <c r="G4" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$G$1,""": """, Requests!D3, """, ", $K$3)</f>
-        <v xml:space="preserve">"Headers": ""Content-Type,": "application/html","Accept,": "*/*"", 
-</v>
-      </c>
-      <c r="H4" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$H$1,""": """, Requests!E3, """, ", $K$3)</f>
-        <v xml:space="preserve">"Request_Body": "{ "JSON" : "Bourne" }", 
-</v>
-      </c>
-      <c r="I4" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$I$1,""": """, Requests!F3, """, ", $K$3)</f>
+      <c r="G3" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$G$1,""": ", Requests!D3, ", ", $K$2)</f>
+        <v xml:space="preserve">"Headers": [{"Name":"Content-Type","Value":"application/html"},{"Name":"Accept","Value":"*/*"}], 
+</v>
+      </c>
+      <c r="H3" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$H$1,""": """, Requests!E3, """, ", $K$2)</f>
+        <v xml:space="preserve">"Request_Body": "{\"JSON\" : \"Bourne\" }", 
+</v>
+      </c>
+      <c r="I3" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$I$1,""": """, Requests!F3, """, ", $K$2)</f>
         <v xml:space="preserve">"Request_Body_FileName": "File_data_to_send.txt", 
 </v>
       </c>
-      <c r="J4" s="3" t="str">
-        <f>_xlfn.CONCAT( """",$J$1,""": """, Requests!G3, """, ", $K$3)</f>
+      <c r="J3" s="3" t="str">
+        <f>_xlfn.CONCAT( """",$J$1,""": """, Requests!G3, """, ", $K$2)</f>
         <v xml:space="preserve">"Output_Filename": "response.txt", 
 </v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
+      <c r="L3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>